<commit_message>
change in BAsetest.java and some new changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>browserName</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>test#kennect.io</t>
-  </si>
-  <si>
-    <t>Qwerty@12345</t>
   </si>
   <si>
     <t>edge</t>
@@ -371,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,7 +376,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -416,13 +410,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -430,18 +424,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -451,12 +445,7 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3" display="test@kennect.io"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="A4" r:id="rId6"/>
-    <hyperlink ref="A5" r:id="rId7" display="test@kennect.io"/>
-    <hyperlink ref="B5" r:id="rId8"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DashBoardTest.java updated and new changes to the BasePage and HomePAge
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D59E3B-7F5F-49D6-B020-D901094153DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId2"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>browserName</t>
   </si>
@@ -45,17 +53,38 @@
     <t>firefox</t>
   </si>
   <si>
-    <t>expectedTest</t>
-  </si>
-  <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>testName</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>Beans</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>UR Uric acid</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>xray</t>
+  </si>
+  <si>
+    <t>expectedTitle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,10 +130,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -378,21 +408,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -400,7 +430,7 @@
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -411,10 +441,10 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -425,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -439,10 +469,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -453,10 +483,10 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -467,16 +497,223 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67F693D1-F121-4984-B0E3-43D565A07370}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{BAE612DC-46EC-4623-81DC-6570F8CEB312}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{2B01B44C-61B7-43E6-825C-C4DA3D7B5A41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EE5FAD7F-B578-4530-95E8-94B5FC059356}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{E029F6D3-DF5D-4522-B136-D33F3DB67818}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A4C5B4CB-0697-4E09-9EF2-88CF76E3B7A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding test page test casess
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D59E3B-7F5F-49D6-B020-D901094153DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C452B-12EF-40CA-9594-44C6E7269BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId2"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId3"/>
+    <sheet name="verifyPageTitle" sheetId="4" r:id="rId2"/>
+    <sheet name="verifyManageTestFunctionality" sheetId="5" r:id="rId3"/>
+    <sheet name="verifyTheSearchResultMatching" sheetId="6" r:id="rId4"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId5"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
   <si>
     <t>browserName</t>
   </si>
@@ -78,6 +81,30 @@
   </si>
   <si>
     <t>expectedTitle</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Manage Tests</t>
+  </si>
+  <si>
+    <t>patientName</t>
+  </si>
+  <si>
+    <t>mike</t>
+  </si>
+  <si>
+    <t>Automated User One</t>
+  </si>
+  <si>
+    <t>fdghgfhfdgh</t>
+  </si>
+  <si>
+    <t>expectedResult</t>
+  </si>
+  <si>
+    <t>pankaj</t>
   </si>
 </sst>
 </file>
@@ -114,12 +141,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -130,11 +172,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -512,11 +556,314 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10FC8CB-4A15-426F-8D4E-E74EA2F78C46}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EDB2C186-E58F-4954-BB1C-AB0F52AC67EF}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{396F2B2E-2E95-480E-97B5-1B8A9401E5B6}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{733D0C12-BAFA-4BCC-9A43-F2D6AA8878BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E701CD-DCBD-47C8-8E53-2BD507AD24A1}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2224DC66-53E7-47F2-A863-6D09885A776F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9D29D226-9C1D-4276-8F6E-99C7A4748692}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{DA31E507-8295-4C4E-929F-C05100603F7D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D994E9F-663D-4EE0-8F77-E85A904780AE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{66EBC12D-F400-49D5-BF9E-8DBB2373D11C}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{011F5100-1674-4325-A8C2-3F869D8913DE}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A142440B-CD3D-4642-A7AA-5629C663C4ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding changes to AddPatientTestcase
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E192A2C1-548D-4DAD-B745-F75F3CFF0D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025BE9D6-FD6B-4B68-851E-AF54CC6A41BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
     <sheet name="verifyPageTitle" sheetId="4" r:id="rId2"/>
     <sheet name="verifyManageTestFunctionality" sheetId="5" r:id="rId3"/>
     <sheet name="verifyTheSearchResultMatching" sheetId="6" r:id="rId4"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId5"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId6"/>
+    <sheet name="verifyAddPatientPageTitle" sheetId="7" r:id="rId5"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId6"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
   <si>
     <t>browserName</t>
   </si>
@@ -105,6 +106,9 @@
   </si>
   <si>
     <t>pankaj</t>
+  </si>
+  <si>
+    <t>Add Patient</t>
   </si>
 </sst>
 </file>
@@ -560,7 +564,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D994E9F-663D-4EE0-8F77-E85A904780AE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,6 +863,102 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD175B6-F2EA-43DE-A2D3-4632EDBE6E66}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B6896989-4BBA-4891-98C5-5953CE970A9A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{BE77B03B-1993-4E1D-B859-62976F7607A8}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E22A459E-B1B1-413C-85EB-82DBF273DBA4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -954,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add patient testcas new update
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025BE9D6-FD6B-4B68-851E-AF54CC6A41BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ACC58B-D322-49AE-96D0-91BA869AA4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="721" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="verifyManageTestFunctionality" sheetId="5" r:id="rId3"/>
     <sheet name="verifyTheSearchResultMatching" sheetId="6" r:id="rId4"/>
     <sheet name="verifyAddPatientPageTitle" sheetId="7" r:id="rId5"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId6"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId7"/>
+    <sheet name="verifyPatientContactDetails" sheetId="8" r:id="rId6"/>
+    <sheet name="verify_WithoutName_TestCase" sheetId="9" r:id="rId7"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId8"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="39">
   <si>
     <t>browserName</t>
   </si>
@@ -109,6 +111,45 @@
   </si>
   <si>
     <t>Add Patient</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>Arnab</t>
+  </si>
+  <si>
+    <t>abc1@gmail.com</t>
+  </si>
+  <si>
+    <t>abc4@gmail.com</t>
+  </si>
+  <si>
+    <t>abc3@gmail.com</t>
+  </si>
+  <si>
+    <t>abc2@gmail.com</t>
+  </si>
+  <si>
+    <t>Hjt</t>
+  </si>
+  <si>
+    <t>HitH</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>expectedMsg</t>
+  </si>
+  <si>
+    <t>Patient name is required</t>
   </si>
 </sst>
 </file>
@@ -866,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD175B6-F2EA-43DE-A2D3-4632EDBE6E66}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,6 +1000,297 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD0A228-C30E-4A37-80B0-857EBBEE2C95}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5052C05A-C9BC-425A-9167-F9631C1AC2DA}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C11252F9-B483-4B31-B196-400F135E0369}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{1DCA5FC6-6FAA-42EE-8891-0649763E0B6B}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{9EE05EAE-07E4-4F22-94AE-F75FE590514C}"/>
+    <hyperlink ref="E3:E5" r:id="rId5" display="abc1@gmail.com" xr:uid="{8D8A5935-C9FD-4DEE-9F9B-0B66481A1EFF}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{8E1BBD0B-2C3D-4501-96F3-32D02038F276}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{61A1BFBD-8FC6-4B68-BDA6-F8D1AF930090}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{E75054E0-29B1-4977-85AD-22D420D2B967}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E566F301-E40B-4AFF-9D21-8D9C6F382F06}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D2:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="4">
+        <v>8956287859</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DD869CD4-29A8-4A72-9C2C-3CAF5E42671F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{40ED1C38-3388-4C08-A53D-0AA1BAFACC85}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{FB605DBC-FDED-4F64-B1FE-9552A90851C6}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{52E7641E-9FD5-4955-8550-E9EA6FD7A534}"/>
+    <hyperlink ref="E3:E5" r:id="rId5" display="abc1@gmail.com" xr:uid="{55CC0BF8-F735-4AF7-A390-0F25FB0D3251}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{5ED47DB5-11C0-4493-A720-40225B1FBE73}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{EA62635A-F5E0-4228-BA27-D521DB05E418}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{45F65304-A5D6-4D71-884D-2F46F9B766A1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -1054,12 +1386,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
starting to add GeneralDetailsTest testcases to the class and some new changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC388D5E-C4DD-4530-8AF7-A3D33DE52CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5C2A2E-702B-4141-966E-0CA028AE8AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="721" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="721" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="verifyAddPatientPageTitle" sheetId="7" r:id="rId5"/>
     <sheet name="verifyPatientContactDetails" sheetId="8" r:id="rId6"/>
     <sheet name="verify_WithoutName_TestCase" sheetId="9" r:id="rId7"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId8"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId9"/>
+    <sheet name="verify_WithoutPhone_TestCase" sheetId="10" r:id="rId8"/>
+    <sheet name="verify_cancelBtn" sheetId="11" r:id="rId9"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId10"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="43">
   <si>
     <t>browserName</t>
   </si>
@@ -150,6 +152,18 @@
   </si>
   <si>
     <t>Patient name is required</t>
+  </si>
+  <si>
+    <t>Arba</t>
+  </si>
+  <si>
+    <t>Payel</t>
+  </si>
+  <si>
+    <t>rimpa</t>
+  </si>
+  <si>
+    <t>Required</t>
   </si>
 </sst>
 </file>
@@ -217,13 +231,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -600,6 +615,213 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{67F693D1-F121-4984-B0E3-43D565A07370}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{BAE612DC-46EC-4623-81DC-6570F8CEB312}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{2B01B44C-61B7-43E6-825C-C4DA3D7B5A41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EE5FAD7F-B578-4530-95E8-94B5FC059356}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{E029F6D3-DF5D-4522-B136-D33F3DB67818}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A4C5B4CB-0697-4E09-9EF2-88CF76E3B7A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10FC8CB-4A15-426F-8D4E-E74EA2F78C46}">
   <dimension ref="A1:D5"/>
@@ -1153,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E566F301-E40B-4AFF-9D21-8D9C6F382F06}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1406,7 @@
       <c r="E1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1205,7 +1427,7 @@
       <c r="E2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>8956287859</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1226,11 +1448,11 @@
       <c r="E3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>8956287859</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,11 +1469,11 @@
       <c r="E4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <v>8956287859</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1268,11 +1490,11 @@
       <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <v>8956287859</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1291,11 +1513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B848F86E-07EA-49DA-A77D-994E3F3BF5F0}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="A1:D6"/>
+      <selection activeCell="G5" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,95 +1525,140 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{67F693D1-F121-4984-B0E3-43D565A07370}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{BAE612DC-46EC-4623-81DC-6570F8CEB312}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{2B01B44C-61B7-43E6-825C-C4DA3D7B5A41}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{71CE6168-078B-442A-B70F-174FF1C8DADA}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{994B8822-C72B-43AE-8875-7DF1253693FF}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{A9483572-09B5-4FF3-AA5A-B844144E4463}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{A4D3FD33-54B2-4AAB-AFD7-504F7F49CE4B}"/>
+    <hyperlink ref="E3:E5" r:id="rId5" display="abc1@gmail.com" xr:uid="{2F5343D3-4903-4011-A947-D9B5217BEABA}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{658F4BC9-13E6-42CE-80D8-7AFF2A344C13}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{CCF267B8-22CF-47CD-8E1F-37AB9AF5610B}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{FFEA8D37-7925-42E1-B9BD-1CC55724A1C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E50ACC-30C7-4C7E-8C7E-89A06FD23E63}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,99 +1666,84 @@
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.05</v>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{EE5FAD7F-B578-4530-95E8-94B5FC059356}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{E029F6D3-DF5D-4522-B136-D33F3DB67818}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{A4C5B4CB-0697-4E09-9EF2-88CF76E3B7A8}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{591E1038-1856-4A8F-8F07-BEB8D74F9EBE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{E3C6C29A-7AEF-4DAF-B599-07D0ECE52F06}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{8704255E-A154-4703-9794-E4534C25DEF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to GenaralDetailsPage and new update on GenaralDetails_TestCases.java file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/LoginData.xlsx
+++ b/src/test/resources/excel/LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Project\GOR_PathologyWeb_AutomationTestong\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5C2A2E-702B-4141-966E-0CA028AE8AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEBDA07-9DEC-4B2E-B38D-6C429D7EFCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="721" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="721" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,9 @@
     <sheet name="verify_WithoutName_TestCase" sheetId="9" r:id="rId7"/>
     <sheet name="verify_WithoutPhone_TestCase" sheetId="10" r:id="rId8"/>
     <sheet name="verify_cancelBtn" sheetId="11" r:id="rId9"/>
-    <sheet name="logedinToDashboard" sheetId="3" r:id="rId10"/>
-    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId11"/>
+    <sheet name="verifySecondaryDetails_positive" sheetId="12" r:id="rId10"/>
+    <sheet name="logedinToDashboard" sheetId="3" r:id="rId11"/>
+    <sheet name="addTestFromDropDown" sheetId="2" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="67">
   <si>
     <t>browserName</t>
   </si>
@@ -164,6 +165,78 @@
   </si>
   <si>
     <t>Required</t>
+  </si>
+  <si>
+    <t>8597525682</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>sys_pressure</t>
+  </si>
+  <si>
+    <t>dia_pressure</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>50</t>
   </si>
 </sst>
 </file>
@@ -616,6 +689,246 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1DAC48-F0B4-4323-8F62-3A6495ADA663}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E64053E3-1BD2-456D-B76F-C6EBE42CF3E3}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B8FED380-71D0-427A-98DA-2D0EF2093125}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{956DE986-358B-43D7-B736-BF8FFACCE4E6}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{B6E905DC-0B0E-4A23-8E8D-AA3A25784793}"/>
+    <hyperlink ref="E3:E5" r:id="rId5" display="abc1@gmail.com" xr:uid="{2BBC7C8C-638D-4096-A544-15A1206B8D78}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{AABF9D11-8467-47B4-9752-9DC91569C72A}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{14B344E4-8AC7-48B1-BEC9-C646F6F6FFBD}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{67B69BB0-D1AB-437A-AE83-2C3B9D542475}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA418E69-62D7-4D6A-B6CC-E2B6E839735F}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -711,7 +1024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2850557C-8B28-470E-8571-E8BAAE419F97}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1376,7 +1689,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:G5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,7 +1970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E50ACC-30C7-4C7E-8C7E-89A06FD23E63}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>